<commit_message>
tpo_placements (version 2 of our project added 2 more features)
</commit_message>
<xml_diff>
--- a/updated_students_data/sheet.xlsx
+++ b/updated_students_data/sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEERA VENKATA RAMANA\Documents\clg_results_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F29BACA-FC29-48A5-9F2C-F3CC7CF59667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FD59D4-9091-4E0F-AF0A-A8189A5F285D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,10 +45,10 @@
     <t>btech_percentage</t>
   </si>
   <si>
-    <t>20NU1A0501</t>
-  </si>
-  <si>
-    <t>ALTHI AISHWARYA</t>
+    <t>20NU1A0503</t>
+  </si>
+  <si>
+    <t>ATTA HARIKA</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -432,7 +432,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -441,13 +441,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="3">
-        <v>9.2100000000000009</v>
+        <v>8.9499999999999993</v>
       </c>
       <c r="E2" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3">
-        <v>84.57</v>
+        <v>82.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>